<commit_message>
fix minor bug on uploading excel on researches
</commit_message>
<xml_diff>
--- a/document/excelResearch.xlsx
+++ b/document/excelResearch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>TITLE</t>
   </si>
@@ -31,84 +31,12 @@
     <t>AUTHOR</t>
   </si>
   <si>
-    <t>WIL Alvarado</t>
-  </si>
-  <si>
-    <t>Joe 2</t>
-  </si>
-  <si>
-    <t>Joe 3</t>
-  </si>
-  <si>
-    <t>Joe 4</t>
-  </si>
-  <si>
-    <t>Joe 5</t>
-  </si>
-  <si>
-    <t>Joe 6</t>
-  </si>
-  <si>
-    <t>Joe 7</t>
-  </si>
-  <si>
-    <t>Joe 8</t>
-  </si>
-  <si>
-    <t>Joe 9</t>
-  </si>
-  <si>
-    <t>Joe 10</t>
-  </si>
-  <si>
-    <t>BBBB</t>
-  </si>
-  <si>
-    <t>TCOS</t>
-  </si>
-  <si>
-    <t>Joe 11</t>
-  </si>
-  <si>
-    <t>Joe 12</t>
-  </si>
-  <si>
-    <t>Joe 13</t>
-  </si>
-  <si>
-    <t>Joe 14</t>
-  </si>
-  <si>
-    <t>Joe 15</t>
-  </si>
-  <si>
-    <t>Joe 16</t>
-  </si>
-  <si>
-    <t>Joe 17</t>
-  </si>
-  <si>
-    <t>Joe 18</t>
-  </si>
-  <si>
-    <t>Joe 19</t>
-  </si>
-  <si>
-    <t>Joe 20</t>
-  </si>
-  <si>
-    <t>joe 1</t>
-  </si>
-  <si>
     <t>TYPE</t>
   </si>
   <si>
     <t>ABSTRACT</t>
   </si>
   <si>
-    <t xml:space="preserve">This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. This is sample from excel. </t>
-  </si>
-  <si>
     <t>thesis</t>
   </si>
   <si>
@@ -116,13 +44,449 @@
   </si>
   <si>
     <t>SCHOOLYEAR</t>
+  </si>
+  <si>
+    <t>This study aims to develop a mobile learning application entitled i-Program: Mobile Learning for Java. The features integrated in the application are all about Java programming language like lessons, terminologies, quizzes and an online compiler for Java programming.
+In system development, deve1opers used Rapid Application Development (RAD). The system used Eclipse with ADT bundles version 4.2.20121004- as its front end. For the system back end, the developers used SQLite. After the system development, evaluation sheets are sent out to actual user and technical users.
+The system was evaluated based on the following criteria: functionality, reliability, usability, portability, speed, and training and documentation. Using the 5 point likert scale, the developers got an overall mean of 4.6 for the acceptability of the system.
+The system is considered as “Excellent” with an average mean of 4.63. Based on the study, the primary conclusion of the developed system helped students, teachers, and future developers to improve their knowledge about Java programming in the easiest way, by using the application i-Program: Mobile Learning for Java.</t>
+  </si>
+  <si>
+    <t>CICT-475IT</t>
+  </si>
+  <si>
+    <t>Reduardo N. Bernardo</t>
+  </si>
+  <si>
+    <t>I-program mobile learning for Java</t>
+  </si>
+  <si>
+    <t>CICT-476IT</t>
+  </si>
+  <si>
+    <t>Damathenics educational damath board game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various mobile games were developed since the advancement of the mobile technology. This gave the researchers to develop “Damathenics: Educational Damath Board Game”, a two player educational board game combining the board game “Dama” and Math. The researchers will implement the game on smartphones and with an Android Operating System environment.
+The objective of the study is to develop an educational and competitive android- based Damath board game that will give the user the convenience of learning while playing. The game would benefit most of the elementary and high school students. The game would be an effective learning tool in teaching mathematics.
+In developing the game, the researchers decided to use the Rapid Application Development Methodology as a based and a guide in building up the game. It is an incremental software process model that focuses on short development cycle time.
+The game was evaluated based on the following criteria: functionality, reliability, usability, maintainability, and portability. Using the 5 point likert scale, the researchers got an overall mean of 4.2 for the acceptability of the game.
+The game is considered as “Very Good” with an average mean of 4.2.
+Based on the study, different conclusions were drawn: (a) The Damathenics: Educational Damath Board Game would be more convenient to learn and play on smartphones and (b) The game needs to meet the hardware and software requirements for it to be able to function properly.
+</t>
+  </si>
+  <si>
+    <t>Alex Paul P. Beriña</t>
+  </si>
+  <si>
+    <t>An android schedule system is the framework of process procedures used to ensure that a college or an organization can fulfill all their schedules and task required to achieve its objective. The android based scheduler system provides encoding of class schedule, meeting schedule, add an announcements and activities, notify the user if there’s a reminder or a message and add the user. It is a Generic system that all colleges that have trouble in generating a schedule can use. It handles all the class schedule, meeting schedule, activities, announcement, messages, notification and profile. Simplistically stated android bases schedule is a methodology needed by those who are responsible in managing schedules.
+In order to make task of managing schedules easier and to eliminate inaccuracy and conflicts encountered in the existing scheduling system. The proponents developed and created the CIC T Mobile Assistant: An Android Task Organizer.
+The C ICT Mobile Assistant: An Android Task replaces the manual process and consolidates all the necessary features to meet the requirements of scheduling. The CICT Mobile app also provides 5 time table to View to the user on selected source and allows switching of resources schedule.
+Schedules that are in conflict with other schedules in the system are not saved, thus minimizing schedule conflicts. A system information is also integrated to the system to provide additional system functionality.</t>
+  </si>
+  <si>
+    <t>CICT mobile assistant android task organizer</t>
+  </si>
+  <si>
+    <t>CICT-477IT</t>
+  </si>
+  <si>
+    <t>Christine Joy M. Delantar</t>
+  </si>
+  <si>
+    <t>The main purpose of the study was to help the graduating students and the repeaters
+of 1 Bulacan State University’s College of Education in preparing for the Licensure
+Examination for Teachers (LET) which was annually held by the Professional Regulation
+Commission (PRC). The study aimed to test their preparedness, helping them know their
+capability and determined their strengths and weaknesses in preparation for the
+examination. Another aim of the study was to help the faculty of the College of Education
+in handling dry-runs exams for the LET, particularly in checking the answers of every
+student.
+In system development, the proponents used Waterfall Method. The proponents
+made use of PHP to conveniently create a user interface and MYSQL to store information
+and questions. After the system development, evaluation sheets are sent out to actual users
+and technical users. Most of them gave a rating of very good in terms of the acceptability
+of the system.
+The output of the system allowed to development of an online LET reviewer. The
+system program served as the examiner for the online exam while the client program served.
+as the examinee. The system program also possessed the checker feature and add it allowed
+report generations. Report made a huge help in terms of monitoring the high ranking and
+the students who need improvement. It also showed the areas where the students are good
+and weak at. 
+The primary conclusion was that the developed system helped the graduating
+students and the repeaters of the College of Education on preparing themselves for the
+actual LET examination and it helped the faculty in handling the online examination.</t>
+  </si>
+  <si>
+    <t>COED online mock examination for teachers</t>
+  </si>
+  <si>
+    <t>CICT-478IT</t>
+  </si>
+  <si>
+    <t>Rickcel A. Alama</t>
+  </si>
+  <si>
+    <t>Patient admission and monitoring system for Jesus the Good Shepherd hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main purpose of the study is to design and develop the Patient Admission and
+Monitoring System for Jesus the Good Shepherd Hospital. The developers transformed the
+existing manual process of the hospital into automated process. Therefore, it will provide ways
+for employees as well patients to communicate and perform transaction in a convenient and
+accessible way.
+The development method that the developers used is to modified scrum model where this
+model is that it is more relaxed approach to formal procedures, documents and reviews. During
+the requirement gathering the developers collected all the essential information and client’s
+suggestion that will act as a. guide and reference of the developers during the development of the
+project. In designing the system, Netbeans IDE 8.0 is plat formed used and Wamp Server for the
+back end database of the system.
+The developers conducted an evaluation testing that will showcase the strength and
+determine the weaknesses of the system. Evaluation testing will help identify possible
+enhancement that can be added to the project. For the level of acceptability of the developed
+software, faculty members of the college and IT professionals evaluated the system using the
+following criteria; functionality, reliability, usability, portability, maintainability and training
+documentation.
+Lastly, based on the findings and conclusions it is recommended that the system must be
+adapted by the hospital which are about to start the automation of their hospital information
+system. For the future developers, it is highly advised that the enhancement of the system
+transactions, report generation and integration of other transactions.
+</t>
+  </si>
+  <si>
+    <t>CICT-479IT</t>
+  </si>
+  <si>
+    <t>Dr. Felipe De Jesus National High School K-12 grading assistant app</t>
+  </si>
+  <si>
+    <t>Smartphones are one of the biggest or widely known technology device that possess the ability to facilitate a task in an instant and in the palm of people’s hand. The success of the open source technology of Android offers much space for customization to the developers. It made the platform to be flexible and handy which attracted the public. Android was the world’s first fully-open complete mobile platform.
+After several research and studies conducted, the developers were able to identify the problem which is how to develop an upgrade in Grading System using android phones. For the development of the applications, developers used Android Studio for the development environment of the application and Java programing as the programming language. The developers assured that the application is user friendly to use and serve as one of the helpful application for the client.
+K-12 Grading Assistant Application for Dr. Felipe National High School. It helps the teacher to minimize the time consume in computing grades of the students. It also focused each underlying technologies used to create and implement the application. And it gives helpful features for the satisfactions of the client. The application will keep the record of the students secured. The computation will be automatically displayed. The teacher will be using this application can make their own schedule of their task in Scheduler tab. Also can create a seat plan using the Seat plan tab Option. In addition, if the teacher forget password, it can still recover by answering the secret question given in creating their account, the application send the whole profile of the user in their email address.</t>
+  </si>
+  <si>
+    <t>CICT-480IT</t>
+  </si>
+  <si>
+    <t>Melanie DC. Fajardo</t>
+  </si>
+  <si>
+    <t>Philippine heroes saga a trading card game</t>
+  </si>
+  <si>
+    <t>The primary objective of this study is to develop an effective card game that teaches the
+players about The Philippine History and Philippine National Heroes. The game also provides
+online multiplayer, strategic game play and virtual battle between the engaged cards. The
+developers gathered and analyzed the data, planned the needs of the game and on how the game
+will work. That can satisfy the player’s knowledge and the capability to understand and enjoy the
+developed game. Therefore, Agile Method was used in order to make this game possible. The
+game was evaluated using the standardized evaluation of the college, following the nine criteria:
+Environment, Concentration, Challenge, Player skills, Control, Clear goals, Feedback, Immersion
+and Social Interaction, the game was evaluated Very Good with overall weighted mean of 4.71.
+This shows that the game is highly accepted for implementation.</t>
+  </si>
+  <si>
+    <t>CICT-481IT</t>
+  </si>
+  <si>
+    <t>Joseph Bello Jr.</t>
+  </si>
+  <si>
+    <t>Web-based project management system for Irizh builders &amp; services, Inc</t>
+  </si>
+  <si>
+    <t>Web-based project management systems are designed to manage and store project
+information that are used in web-based applications. To increase an efficiency of a product,
+nowadays many web development companies are using different project management systems.
+The aim of the project was to make complete, fully working web based project management system
+for lrizh Builders &amp; Services Incorporated. The most important requirements are to integrate
+project and schedule managing, generate reports, messaging, creating task and changing orders.
+The developers used Agile Methodology because it is much faster, more effective and
+accurate method for the developed system. Agile Methodology provides transparency, early and
+predictable delivery, predictable costs and schedule, allows for change focuses on customer’s
+needs and improves quality. The developers used a tool such as Google chrome browser, since
+web-based applications the system can be accessed through any browser.
+To conclude, web-based project management system was developed for the client to
+improve productivity and efficiency of managing projects. The result of the developed system
+responded to the customer’s expectation. The IBI was satisfied with the features developed and
+the reliability and robustness. The IBI web-based project management system was completed as
+one fully functioning system that corresponds to the company’s needs.</t>
+  </si>
+  <si>
+    <t>CICT-482IT</t>
+  </si>
+  <si>
+    <t>John Omar B. Azada</t>
+  </si>
+  <si>
+    <t>Online reservation system for GJ's catering and services</t>
+  </si>
+  <si>
+    <t>This study aims to develop and design the Online Reservation System for GJ’s
+Catering and Services. It presents features that can be used easily and familiarize clients
+on the online reservation system, evaluate it, and highlight the benefits it can provide to
+the customers and staff. In addition, It will provide supplement material in their front
+desk operation course. The developers used the Agile Scrum Methodology including
+Web Development PHP, HTML 5, CSS 3, MySQL, Javascript as their scripting
+language. The developed software served as a tool for the customer and the administrator
+of the catering services to familiarize them on how to Operate an online reservation
+system. The developed software was an effective aid for the secretary and administrator
+in the basic operation of online reservation system. It also provides online security to
+protect privacy and financial information of the customers and served as the administrator
+side of online reservation system that can accept and cancel reservation, and edit package
+information. It also includes the customization of package where the customer can choose
+the desired menus the customers wants.</t>
+  </si>
+  <si>
+    <t>CICT-483IT</t>
+  </si>
+  <si>
+    <t>Leonida B. Cuevo</t>
+  </si>
+  <si>
+    <t>Online reservation website for RDM express travel and tour</t>
+  </si>
+  <si>
+    <t>The developers created an Online Reservation Website for RDM Express Travel
+and Tour for the advertisement and reservation of the business of our client Mr. Rodel D.
+Martinez.
+The objectives of the developed website is to advertise and promote our client’s
+business and have reservation process through the website. The developed website have 3
+user level access (a) Guest Customer, (b) Registered Customer and (c) Administrator.
+Each user level access have different function that will be discussed at the scope and
+delimitation section. of the study.
+The developers used the development method called System Development Life
+Cycle (SDLC) which are used by system engineers and system developers. This
+development method comprised of six phases: (1) Planning Phase, (2) Analysis Phase, (3)
+Design Phase, (4) Development Phase, (5) Testing Phase, (6) Maintenance Phase.
+The project was evaluated using 5 point scale &amp; have the following my)
+functionality, the average mean of 4.44 which is considered as "acceptable"
+Reliability, the average mean of 4.17 which is considered as “Slightly Acceptable"
+Usability, the average mean of 4.45 which is considered as “Acceptable"
+Maintainability, the average mean of 4.32 which is considered as, "Acceptable"
+Portability, the average mean of 4.30 which is considered as “Acceptable".</t>
+  </si>
+  <si>
+    <t>CICT-484IT</t>
+  </si>
+  <si>
+    <t>Ana Lyn M. Bondoc</t>
+  </si>
+  <si>
+    <t>Online Public Access Catalog for local Research Offices of Bulacan State University</t>
+  </si>
+  <si>
+    <t>The project mainly focuses on the development of an Online Public Access Catalog for
+Local Research Offices, particularly for Bulacan State University. The study aims to provide a
+reliable access to the studies and researches for researchers and to provide a tool for management
+of studies and researches with ease of operation in mind. The Online Public Access Catalog for
+Local Research Offices of Bulacan State University covers the creation and uploading of thesis
+titles in the database, retrieval of thesis titles and its information, full management of thesis titles
+in the database- user management, and the generation of reports.
+The project is developed by using an agile methodology as its software development
+model, particularly, Scrum because it support based on the empirical research as theory. The
+software development model used by the developers is perfectly fit for the ever changing
+requirements of the client. The developers also used PHP for back-end programming, MySQL
+for database and HTML and CSS for front-end design.
+It came to the conclusion with the aim of the system by ensuring organized database
+collection of abstract will be kept and stored in a secure database, making the data storage
+management more credible and reliable.</t>
+  </si>
+  <si>
+    <t>CICT-485IT</t>
+  </si>
+  <si>
+    <t>Mark Christian DV. Bautista</t>
+  </si>
+  <si>
+    <t>Grade recorder and faculty evaluation for Holy Angels Colleges of Pulilan</t>
+  </si>
+  <si>
+    <t>This Capstone Project aims to develop a Grade Recorder and
+Faculty Evaluation for Holy Angels Colleges of Pulilan. The features
+integrated in the website are online evaluation, online grading system, and
+posting of announcements and events. This study is useful for the HACP
+because it improves the manual process of the school.
+The website used Sublime text 3.0 as its front end and for the
+system’s back end the developers used Apache Server.
+The System was evaluated based on the following criteria:
+Functionality, Reliability, Usability, Maintainability and Portability. Using
+the 5 point highest scale, the researchers got an overall mean of 4.14 for
+the acceptability of the system as considered as “Very Good”.
+Based on the study, different conclusion were drawn: (a) The
+Grade Recorder and Faculty Evaluation for HACP needs a website for
+advertising the school and to transfer all the manual process into online
+process. (b) The website needs to meet the hardware and software
+requirements for it to be able to function properly.
+Lastly, based on the findings and conclusions, it is recommended
+that the website must be adapted by the school which are about to start the
+automation of their online procedures. For future researchers, it is highly 
+advised that the enhancements of website is to have viewing of payments
+forum, security purpose and integration of other menus and other tools.</t>
+  </si>
+  <si>
+    <t>CICT-486IT</t>
+  </si>
+  <si>
+    <t>Melvin DJ. Estrella</t>
+  </si>
+  <si>
+    <t>Juan direction a mobile city guide for Central Luzon</t>
+  </si>
+  <si>
+    <t>Nowadays, mobile phone is a necessary part of the people’s life. The goal of the
+project is to develop an application that acts as an endeavor to help travelers in finding
+places to visit. giving directional assistance and will give the local and foreign tourist a
+background information about a particular location.
+The project uses Agile Development Process. Through planning, designing,
+development and quality assurance. the goal of the project is reached.
+The developed project functionalities when offline mode includes showing user’s
+current location from the map. search location, routing of walk, drive and bike and
+viewing of nearby categories on user‘s current location such as: food, sights,
+transportation, hotel, gas station, school, entertainment, shop, automated teller machine
+(ATM), Bank, hospital. pharmacy and police station including its profile viewing.
+However, these features are still available when online mode plus user can submit
+reviews such as: rate, Comment, upload photo comment and picking favorite.
+Overall. the project is a new built android application that is going to be a guide
+for everyone especially for the tourists who are not familiar with Central Luzon.</t>
+  </si>
+  <si>
+    <t>CICT-487IT</t>
+  </si>
+  <si>
+    <t>Regina Carmella S. Antonis</t>
+  </si>
+  <si>
+    <t>Y.M.Lopez web-based sales and purchasing system</t>
+  </si>
+  <si>
+    <t>The Y.M.Lopez Web Based Sales and Purchasing System was developed for the
+advertising the hardware store. It promotes convenience for the both customer
+while decreases employees expenses. It also help to promote their business through the world wide web because nowadays, one way to introduce something or someone is to be in the "cyber space”.
+There are different ways to gather information for this project for it to be reliable and functional because it is one of the most important aspects of giving information to the 
+customers. It Will help the business to commercialize more their products by advertising through its own site and at the same time the customers can order even though they are far from the store. Significantly, the system’s main features are the following.
+The website encourages the viewers to register for an account in order to purchase the products in the website. The registered users can also edit its own account information and also view the transactions history.
+In developing the project, the researchers made use of the Iterative waterfall model.
+The Iterative waterfall model helps the researchers in building and improving the website step by step. 
+This model helps the researchers to track the defects at the early ages and avoids the downward flow of the defects.
+In terms of evaluation, the project was evaluated according to its acceptability based
+on the following criteria: Authority; Purpose; Currency; Objectivity; Accuracy;
+Functionality; and Training and Documentation. The overall weighted mean has a scale of
+4.19 which characterizes as “Very Good”. This means that the website developed is
+acceptable and recommended for further improvement.</t>
+  </si>
+  <si>
+    <t>CICT-488IT</t>
+  </si>
+  <si>
+    <t>Jerome S. Dayog</t>
+  </si>
+  <si>
+    <t>BulSU web-based alumni information system</t>
+  </si>
+  <si>
+    <t>The main purpose of this study is to design and develop a “BulSU Web-based Alumni Management Information System” that serves as an online graduate communication site for the university and also to eliminate the redundancy of the information of every alumnus.
+The website is allowing old and fresh students of the university or college to interconnect with each other. This will allow students to know about each other and present activities. Alumni Information System is set up and synchronizes alumni activities which lead to much closer connections between the university and their alumni.
+The developed project is useful and helpful for the BulSU Alumni office and Alumni Director and to future developer because it will lessen the time consumed in tracing the graduates, provide the BulSU Alumnus a medium of communication and at the same time, serve as a pathway for agencies/companies in viewing the profile of the BulSU graduates.
+The features integrated in the website are Forums, Upload photos, News and events page, message, and admin feedback. You can see the history of alumni and the university in the home page of the alumni.</t>
+  </si>
+  <si>
+    <t>CICT-489IT</t>
+  </si>
+  <si>
+    <t>Henesie S. Alday</t>
+  </si>
+  <si>
+    <t>Cobalt Argyros VR using Google Cardboard</t>
+  </si>
+  <si>
+    <t>Virtual Reality VR and its technical support drivers is first described, then applications that drive VR are listed together with engineering design features. A basic theme is that normal vision depends upon a set of perceptual Visual illusions, such as continuity and 3D-ness of the world, and that these work equally well in virtual environments. An important visual illusion, that of the completeness and clarity of our visual world, must be a top-down perceptual phenomenon and is explicable on the basis of the scan path theory. This theory states that active looking and perception are controlled by an internal cognitive model. New evidence for this control of the sparse sampling in time and space of the visual world comes from visual imagery experiments; quantitative methods for assessment have been developed. Finally, perceptual philosophical thought is used to situate this new scientific evidence.
+The game Virtual reality VR is a technology which allows a user to interact with a computer-simulated environment, whether that environment is a simulation of the real world or an imaginary world. It is the key to experiencing, feeling and touching the past, present and the future. It is the medium of creating our own world, our own customized reality. It could range from creating a video game to having a virtual stroll around the universe, from walking through our own dream house to experiencing a walk on an alien planet. With virtual reality, we can experience the most intimidating and grueling situations by playing safe and with a learning perspective.
+Mobile gaming industry is well- developed and there are wide ranges of games which can be played on the mobile easily. Android games development is getting rapid growth as mobile game in industry is blooming.</t>
+  </si>
+  <si>
+    <t>CICT-490IT</t>
+  </si>
+  <si>
+    <t>Ramil P. Anson</t>
+  </si>
+  <si>
+    <t>BulSU guidance counseling information system</t>
+  </si>
+  <si>
+    <t>This study aims to develop a web application information system for BulSU Guidance Services Center. The features integrated in the system will enhance the quality of the guidance service by providing and maintaining accurate records and speeding up the mode of information keeping procedure.
+The system needs to meet the user requirements in order for it to be able to function properly. User requirements include recording and generating reports.
+The system used HTML, CSS as its front end. For the system back end, PHP, JQuery and Ajax are used.
+The system was evaluated based on the following criteria: functionality, reliability, usability, maintainability and portability. Using the 5 point Likert scale, the total rating for the final system evaluation is 4.45, equivalent to a rating of Very Good.
+The system received high evaluation rating, making the system more likely to be implemented by the client; High ratings from the clientele signify eager approval of this system.
+The researchers have concluded that the system objectives were met. The system has the fill capability of keeping track of records. Upon the implementation of the system, the researchers come up with the idea of some recommendations for the improvement of the related future studies. Future researchers may consider enhancement in recording and generating reports also an integration of some menus and functionalities.</t>
+  </si>
+  <si>
+    <t>CICT-491IT</t>
+  </si>
+  <si>
+    <t>Rose Anne Benedictos</t>
+  </si>
+  <si>
+    <t>BulSU pathfinder</t>
+  </si>
+  <si>
+    <t>This study aims to be a three dimensional map for Bulacan State University main campus where you can search a specific building and rooms. The application allows the users to see the environment of the University and a particular place in 3D, with the added ability to rotate and tilt the angle in addition to panning and zooming. This study is useful most especially for those incoming freshmen students and for anyone who are not 1familiar with the school facilities. The system will lessen the time spent in searching for a precise building or room in Bulacan State University main campus.
+The developers used Google Sketch Up for making 3D models. Then Unity 3D for programming platform, both are IDE for android development, and SDK for android development also.
+The application was evaluated based of the following criteria: Functionality, Reliability, Usability, Maintainability, Portability, and Training and Documentation. Using likert scale, the developers got an overall mean of 4.79 and therefore, the application is considered as “Excellent”.
+Based on the findings and conclusions, doing something completely new is proved to be challenging but it also helped us to be more acquainted to Bulacan State University. For future researchers, think of something useful to add and will be efficient for the user, get all the information you needed about the school, facilities, and colleges. If you have to use an environment that you are not familiar with, you must study and research all the things you need. Doing a study using software that is new to you is also good because you have a chance to learn something new, and discover things that you are not familiar with.</t>
+  </si>
+  <si>
+    <t>CICT-492IT</t>
+  </si>
+  <si>
+    <t>Adison S. Aliwalas</t>
+  </si>
+  <si>
+    <t>CICT anti-plagiarism software (web-based)</t>
+  </si>
+  <si>
+    <t>The rising number of plagiarised documents, theses, home works, and projects is a major issue to be solved. The study aims to improve the quality of documents being made by the bachelor of information technology students. The CICT Anti-Plagiarism Software detects if the document is certified copy pasted or plagiarised. The system helps in promoting the student’s integrity in developing the student’s ability to write or compose ideas and most importantly, thesis documentations.
+The system is web-based which means it requires internet access to run and be used. The users are exclusively for CICT teaching personnel and students. The system requires the user to login before enjoying the services for free.
+The user can easily use the system after successful registration. The main function of the system is to detect if the document is plagiarised. This is done by simply copy/pasting the document on the search box and clicking the button “Search”. The system then, will display a report. Another function is, the contributing author can also manage the documents which means they can add new document. Added documents which are saved on the database can now serve as a reference for matching documents.
+The project was developed using Notepad++ as the platform for the coding. The proponents used programming languages such as: html, php, javascript, and 083. The local database server used is Wamp Server, XAMPP, and for the database is MySQL.</t>
+  </si>
+  <si>
+    <t>CICT-493IT</t>
+  </si>
+  <si>
+    <t>Rosel DL. Aresala</t>
+  </si>
+  <si>
+    <t>Knowledge-based medical diagnostic guide</t>
+  </si>
+  <si>
+    <t>The main purpose of this study is to develop an “Knowledge-based Medical Diagnostic Guide“ intended for people in the Philippines.
+Functions like: (a) viewing of illness information; (b) capable of implementing knowledge by medical diagnostic guide; and (c) updating of medical condition information are incorporated in the system.
+For system requirements, software specification requires using Notepad++ and Xampp for handling the database application and hardware Specification recommend to use CORE13 Processor, 4gb RAM and 500gb HDD Intel Graphics 4400.
+Software Development Life Cycle (Agile Model) was used in the development of the system.
+The constraints of the system are: (a) guests cannot log in to the system; (b) users cannot secure a softcopy of images and textual information being provided in the system; and (c) it does not generate laboratory forms by any means.
+The conclusions in this learning are: (1) This study developed a system that enhance the service in a society and provide additional medical and health knowledge and information through medical diagnostic guide; and (2) Only the administrator is authorized to handle the updating and overall management of records.
+The recommendations in this learning are: (1) Users should have a right to acquire a softcopy of images and textual information in the system through a download for them to study every details; and (2) The future developers can develop a system where their knowledge suited the best especially in using other programming languages.</t>
+  </si>
+  <si>
+    <t>CICT-494IT</t>
+  </si>
+  <si>
+    <t>Jamell Rose A. De Vera</t>
+  </si>
+  <si>
+    <t>College of Information and Communications Technology</t>
+  </si>
+  <si>
+    <t>Bachelor of Science in Information Technology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +522,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -189,7 +559,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,21 +869,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -519,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -528,599 +901,599 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2016</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2016</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2016</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2">
-        <v>123</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>40513</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2">
-        <v>123</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>40513</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2">
-        <v>123</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>40513</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2">
-        <v>123</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>40513</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2">
-        <v>123</v>
+      <c r="F6" t="s">
+        <v>28</v>
       </c>
       <c r="G6" s="2">
         <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="2">
-        <v>123</v>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2">
-        <v>123</v>
+        <v>34</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2">
-        <v>123</v>
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
       </c>
       <c r="H9" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2">
-        <v>123</v>
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2">
-        <v>123</v>
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G11" s="2">
         <v>2</v>
       </c>
       <c r="H11" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="2">
-        <v>123</v>
+        <v>50</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="2">
         <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="2">
-        <v>123</v>
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="G13" s="2">
         <v>2</v>
       </c>
       <c r="H13" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="2">
-        <v>123</v>
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
       <c r="H14" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="2">
-        <v>123</v>
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G15" s="2">
         <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="2">
-        <v>123</v>
+        <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
       <c r="H16" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2">
-        <v>123</v>
+        <v>70</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="G17" s="2">
         <v>2</v>
       </c>
       <c r="H17" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2">
-        <v>123</v>
+        <v>74</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="G18" s="2">
         <v>2</v>
       </c>
       <c r="H18" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2">
-        <v>123</v>
+        <v>78</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G19" s="2">
         <v>2</v>
       </c>
       <c r="H19" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="2">
-        <v>123</v>
+        <v>82</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="G20" s="2">
         <v>2</v>
       </c>
       <c r="H20" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2">
-        <v>123</v>
+        <v>86</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="G21" s="2">
         <v>2</v>
       </c>
       <c r="H21" s="2">
-        <v>40513</v>
+        <v>2016</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>